<commit_message>
fixed a crash bug
</commit_message>
<xml_diff>
--- a/DataImport/Timeseries/ImportFromSentekIrrimaxWeb/Configuration.xlsx
+++ b/DataImport/Timeseries/ImportFromSentekIrrimaxWeb/Configuration.xlsx
@@ -60,10 +60,10 @@
     <t>last hours to import</t>
   </si>
   <si>
-    <t>If FALSE, import data in time interval &lt;from_time&gt; to &lt;to_time&gt;. Use for initial import of large data sets. If TRUE, import the last x hours, where x = &lt;relative offset&gt;. Use this option for continuous updates.</t>
-  </si>
-  <si>
     <t>!!! Set API key in Spreadsheet!!!</t>
+  </si>
+  <si>
+    <t>If FALSE, import data in time interval &lt;from_time&gt; to &lt;to_time&gt;. Use for initial import of large data sets (if getting HTTPErrors, reduce the time intervall). If TRUE, import the last x hours, where x = &lt;relative offset&gt;. Use this option for continuous updates.</t>
   </si>
 </sst>
 </file>
@@ -546,7 +546,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +569,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
@@ -608,7 +608,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -616,7 +616,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>